<commit_message>
Updated monthly Honorable Rock
</commit_message>
<xml_diff>
--- a/data/MapleStory Monthly Honorable Rock Record.xlsx
+++ b/data/MapleStory Monthly Honorable Rock Record.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="August 2019" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="September 2019" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="October 2019" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="November 2019" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="54">
   <si>
     <t xml:space="preserve">Rank</t>
   </si>
@@ -446,7 +447,7 @@
   </sheetPr>
   <dimension ref="B1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
@@ -1267,7 +1268,7 @@
   </sheetPr>
   <dimension ref="B1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -2088,7 +2089,7 @@
   </sheetPr>
   <dimension ref="B1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2900,4 +2901,825 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:E54"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="0.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="59.9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="4.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="str">
+        <f aca="false">"    """&amp;"November 2019"&amp;""""&amp;":"</f>
+        <v>    "November 2019":</v>
+      </c>
+    </row>
+    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="10" t="str">
+        <f aca="false">"    "&amp;"["</f>
+        <v>    [</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12" t="n">
+        <v>237814795</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f aca="false">"      "&amp;"{""rank"": "&amp;B4&amp;", ""name"": """&amp;C4&amp;""", ""contribution"": "&amp;D4&amp;"}"</f>
+        <v>      {"rank": 1, "name": "Eternal", "contribution": 237814795}</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="12" t="n">
+        <v>222924716</v>
+      </c>
+      <c r="E5" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B5&amp;", ""name"": """&amp;C5&amp;""", ""contribution"": "&amp;D5&amp;"}"</f>
+        <v>      , {"rank": 2, "name": "Smile", "contribution": 222924716}</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="12" t="n">
+        <v>206424668</v>
+      </c>
+      <c r="E6" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B6&amp;", ""name"": """&amp;C6&amp;""", ""contribution"": "&amp;D6&amp;"}"</f>
+        <v>      , {"rank": 3, "name": "Savages", "contribution": 206424668}</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12" t="n">
+        <v>202612882</v>
+      </c>
+      <c r="E7" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B7&amp;", ""name"": """&amp;C7&amp;""", ""contribution"": "&amp;D7&amp;"}"</f>
+        <v>      , {"rank": 4, "name": "Elite", "contribution": 202612882}</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="12" t="n">
+        <v>195124955</v>
+      </c>
+      <c r="E8" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B8&amp;", ""name"": """&amp;C8&amp;""", ""contribution"": "&amp;D8&amp;"}"</f>
+        <v>      , {"rank": 5, "name": "Bounce", "contribution": 195124955}</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="12" t="n">
+        <v>146174652</v>
+      </c>
+      <c r="E9" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B9&amp;", ""name"": """&amp;C9&amp;""", ""contribution"": "&amp;D9&amp;"}"</f>
+        <v>      , {"rank": 6, "name": "Spring", "contribution": 146174652}</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="12" t="n">
+        <v>134839967</v>
+      </c>
+      <c r="E10" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B10&amp;", ""name"": """&amp;C10&amp;""", ""contribution"": "&amp;D10&amp;"}"</f>
+        <v>      , {"rank": 7, "name": "Sunset", "contribution": 134839967}</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="12" t="n">
+        <v>119673264</v>
+      </c>
+      <c r="E11" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B11&amp;", ""name"": """&amp;C11&amp;""", ""contribution"": "&amp;D11&amp;"}"</f>
+        <v>      , {"rank": 8, "name": "Epic", "contribution": 119673264}</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="12" t="n">
+        <v>113365977</v>
+      </c>
+      <c r="E12" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B12&amp;", ""name"": """&amp;C12&amp;""", ""contribution"": "&amp;D12&amp;"}"</f>
+        <v>      , {"rank": 9, "name": "Downtime", "contribution": 113365977}</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="12" t="n">
+        <v>112448493</v>
+      </c>
+      <c r="E13" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B13&amp;", ""name"": """&amp;C13&amp;""", ""contribution"": "&amp;D13&amp;"}"</f>
+        <v>      , {"rank": 10, "name": "Beaters", "contribution": 112448493}</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="12" t="n">
+        <v>99249305</v>
+      </c>
+      <c r="E14" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B14&amp;", ""name"": """&amp;C14&amp;""", ""contribution"": "&amp;D14&amp;"}"</f>
+        <v>      , {"rank": 11, "name": "RainSong", "contribution": 99249305}</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="12" t="n">
+        <v>96254842</v>
+      </c>
+      <c r="E15" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B15&amp;", ""name"": """&amp;C15&amp;""", ""contribution"": "&amp;D15&amp;"}"</f>
+        <v>      , {"rank": 12, "name": "Imperium", "contribution": 96254842}</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="11" t="n">
+        <v>13</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="12" t="n">
+        <v>96210291</v>
+      </c>
+      <c r="E16" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B16&amp;", ""name"": """&amp;C16&amp;""", ""contribution"": "&amp;D16&amp;"}"</f>
+        <v>      , {"rank": 13, "name": "lolicafe", "contribution": 96210291}</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="12" t="n">
+        <v>86205385</v>
+      </c>
+      <c r="E17" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B17&amp;", ""name"": """&amp;C17&amp;""", ""contribution"": "&amp;D17&amp;"}"</f>
+        <v>      , {"rank": 14, "name": "Gintama", "contribution": 86205385}</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="12" t="n">
+        <v>85678663</v>
+      </c>
+      <c r="E18" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B18&amp;", ""name"": """&amp;C18&amp;""", ""contribution"": "&amp;D18&amp;"}"</f>
+        <v>      , {"rank": 15, "name": "Undertale", "contribution": 85678663}</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="12" t="n">
+        <v>82758780</v>
+      </c>
+      <c r="E19" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B19&amp;", ""name"": """&amp;C19&amp;""", ""contribution"": "&amp;D19&amp;"}"</f>
+        <v>      , {"rank": 16, "name": "Remorse", "contribution": 82758780}</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="12" t="n">
+        <v>82327678</v>
+      </c>
+      <c r="E20" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B20&amp;", ""name"": """&amp;C20&amp;""", ""contribution"": "&amp;D20&amp;"}"</f>
+        <v>      , {"rank": 17, "name": "Maha", "contribution": 82327678}</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="12" t="n">
+        <v>80545548</v>
+      </c>
+      <c r="E21" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B21&amp;", ""name"": """&amp;C21&amp;""", ""contribution"": "&amp;D21&amp;"}"</f>
+        <v>      , {"rank": 18, "name": "Erda", "contribution": 80545548}</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="11" t="n">
+        <v>19</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="12" t="n">
+        <v>78049625</v>
+      </c>
+      <c r="E22" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B22&amp;", ""name"": """&amp;C22&amp;""", ""contribution"": "&amp;D22&amp;"}"</f>
+        <v>      , {"rank": 19, "name": "Atelier", "contribution": 78049625}</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="12" t="n">
+        <v>75168538</v>
+      </c>
+      <c r="E23" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B23&amp;", ""name"": """&amp;C23&amp;""", ""contribution"": "&amp;D23&amp;"}"</f>
+        <v>      , {"rank": 20, "name": "Sora", "contribution": 75168538}</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="11" t="n">
+        <v>21</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="12" t="n">
+        <v>74658941</v>
+      </c>
+      <c r="E24" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B24&amp;", ""name"": """&amp;C24&amp;""", ""contribution"": "&amp;D24&amp;"}"</f>
+        <v>      , {"rank": 21, "name": "Cleanse", "contribution": 74658941}</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="11" t="n">
+        <v>22</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="12" t="n">
+        <v>73544475</v>
+      </c>
+      <c r="E25" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B25&amp;", ""name"": """&amp;C25&amp;""", ""contribution"": "&amp;D25&amp;"}"</f>
+        <v>      , {"rank": 22, "name": "Broke", "contribution": 73544475}</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="12" t="n">
+        <v>72353558</v>
+      </c>
+      <c r="E26" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B26&amp;", ""name"": """&amp;C26&amp;""", ""contribution"": "&amp;D26&amp;"}"</f>
+        <v>      , {"rank": 23, "name": "Tama", "contribution": 72353558}</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="12" t="n">
+        <v>68755618</v>
+      </c>
+      <c r="E27" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B27&amp;", ""name"": """&amp;C27&amp;""", ""contribution"": "&amp;D27&amp;"}"</f>
+        <v>      , {"rank": 24, "name": "Oceania", "contribution": 68755618}</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="12" t="n">
+        <v>65982830</v>
+      </c>
+      <c r="E28" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B28&amp;", ""name"": """&amp;C28&amp;""", ""contribution"": "&amp;D28&amp;"}"</f>
+        <v>      , {"rank": 25, "name": "Lithe", "contribution": 65982830}</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="11" t="n">
+        <v>26</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="12" t="n">
+        <v>65235043</v>
+      </c>
+      <c r="E29" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B29&amp;", ""name"": """&amp;C29&amp;""", ""contribution"": "&amp;D29&amp;"}"</f>
+        <v>      , {"rank": 26, "name": "Revive", "contribution": 65235043}</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="11" t="n">
+        <v>27</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="12" t="n">
+        <v>62360160</v>
+      </c>
+      <c r="E30" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B30&amp;", ""name"": """&amp;C30&amp;""", ""contribution"": "&amp;D30&amp;"}"</f>
+        <v>      , {"rank": 27, "name": "Ravers", "contribution": 62360160}</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="11" t="n">
+        <v>28</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="12" t="n">
+        <v>61904014</v>
+      </c>
+      <c r="E31" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B31&amp;", ""name"": """&amp;C31&amp;""", ""contribution"": "&amp;D31&amp;"}"</f>
+        <v>      , {"rank": 28, "name": "Rising", "contribution": 61904014}</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="11" t="n">
+        <v>29</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="12" t="n">
+        <v>61854383</v>
+      </c>
+      <c r="E32" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B32&amp;", ""name"": """&amp;C32&amp;""", ""contribution"": "&amp;D32&amp;"}"</f>
+        <v>      , {"rank": 29, "name": "Sugar", "contribution": 61854383}</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="12" t="n">
+        <v>61167779</v>
+      </c>
+      <c r="E33" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B33&amp;", ""name"": """&amp;C33&amp;""", ""contribution"": "&amp;D33&amp;"}"</f>
+        <v>      , {"rank": 30, "name": "Artifacts", "contribution": 61167779}</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="11" t="n">
+        <v>31</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="12" t="n">
+        <v>55097872</v>
+      </c>
+      <c r="E34" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B34&amp;", ""name"": """&amp;C34&amp;""", ""contribution"": "&amp;D34&amp;"}"</f>
+        <v>      , {"rank": 31, "name": "Fabled", "contribution": 55097872}</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="11" t="n">
+        <v>32</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="12" t="n">
+        <v>53616057</v>
+      </c>
+      <c r="E35" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B35&amp;", ""name"": """&amp;C35&amp;""", ""contribution"": "&amp;D35&amp;"}"</f>
+        <v>      , {"rank": 32, "name": "Aloe", "contribution": 53616057}</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="11" t="n">
+        <v>33</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="12" t="n">
+        <v>50461914</v>
+      </c>
+      <c r="E36" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B36&amp;", ""name"": """&amp;C36&amp;""", ""contribution"": "&amp;D36&amp;"}"</f>
+        <v>      , {"rank": 33, "name": "Earnest", "contribution": 50461914}</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="11" t="n">
+        <v>34</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="12" t="n">
+        <v>49672252</v>
+      </c>
+      <c r="E37" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B37&amp;", ""name"": """&amp;C37&amp;""", ""contribution"": "&amp;D37&amp;"}"</f>
+        <v>      , {"rank": 34, "name": "Skyfall", "contribution": 49672252}</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="11" t="n">
+        <v>35</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="12" t="n">
+        <v>48991344</v>
+      </c>
+      <c r="E38" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B38&amp;", ""name"": """&amp;C38&amp;""", ""contribution"": "&amp;D38&amp;"}"</f>
+        <v>      , {"rank": 35, "name": "CyberThreat", "contribution": 48991344}</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="11" t="n">
+        <v>36</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="12" t="n">
+        <v>48972339</v>
+      </c>
+      <c r="E39" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B39&amp;", ""name"": """&amp;C39&amp;""", ""contribution"": "&amp;D39&amp;"}"</f>
+        <v>      , {"rank": 36, "name": "chigga", "contribution": 48972339}</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="11" t="n">
+        <v>37</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="12" t="n">
+        <v>47766075</v>
+      </c>
+      <c r="E40" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B40&amp;", ""name"": """&amp;C40&amp;""", ""contribution"": "&amp;D40&amp;"}"</f>
+        <v>      , {"rank": 37, "name": "Mystical", "contribution": 47766075}</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="11" t="n">
+        <v>38</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="12" t="n">
+        <v>46803556</v>
+      </c>
+      <c r="E41" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B41&amp;", ""name"": """&amp;C41&amp;""", ""contribution"": "&amp;D41&amp;"}"</f>
+        <v>      , {"rank": 38, "name": "Fandom", "contribution": 46803556}</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="11" t="n">
+        <v>39</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D42" s="12" t="n">
+        <v>45036671</v>
+      </c>
+      <c r="E42" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B42&amp;", ""name"": """&amp;C42&amp;""", ""contribution"": "&amp;D42&amp;"}"</f>
+        <v>      , {"rank": 39, "name": "Path", "contribution": 45036671}</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="11" t="n">
+        <v>40</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="12" t="n">
+        <v>44448074</v>
+      </c>
+      <c r="E43" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B43&amp;", ""name"": """&amp;C43&amp;""", ""contribution"": "&amp;D43&amp;"}"</f>
+        <v>      , {"rank": 40, "name": "Comity", "contribution": 44448074}</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="11" t="n">
+        <v>41</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="12" t="n">
+        <v>43668039</v>
+      </c>
+      <c r="E44" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B44&amp;", ""name"": """&amp;C44&amp;""", ""contribution"": "&amp;D44&amp;"}"</f>
+        <v>      , {"rank": 41, "name": "Howl", "contribution": 43668039}</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="11" t="n">
+        <v>42</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="12" t="n">
+        <v>42657720</v>
+      </c>
+      <c r="E45" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B45&amp;", ""name"": """&amp;C45&amp;""", ""contribution"": "&amp;D45&amp;"}"</f>
+        <v>      , {"rank": 42, "name": "Bubbles", "contribution": 42657720}</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="11" t="n">
+        <v>43</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="12" t="n">
+        <v>42494732</v>
+      </c>
+      <c r="E46" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B46&amp;", ""name"": """&amp;C46&amp;""", ""contribution"": "&amp;D46&amp;"}"</f>
+        <v>      , {"rank": 43, "name": "Coffee", "contribution": 42494732}</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="11" t="n">
+        <v>44</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="12" t="n">
+        <v>42203249</v>
+      </c>
+      <c r="E47" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B47&amp;", ""name"": """&amp;C47&amp;""", ""contribution"": "&amp;D47&amp;"}"</f>
+        <v>      , {"rank": 44, "name": "RainDrop", "contribution": 42203249}</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" s="12" t="n">
+        <v>41811578</v>
+      </c>
+      <c r="E48" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B48&amp;", ""name"": """&amp;C48&amp;""", ""contribution"": "&amp;D48&amp;"}"</f>
+        <v>      , {"rank": 45, "name": "Weibo", "contribution": 41811578}</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="11" t="n">
+        <v>46</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D49" s="12" t="n">
+        <v>41143753</v>
+      </c>
+      <c r="E49" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B49&amp;", ""name"": """&amp;C49&amp;""", ""contribution"": "&amp;D49&amp;"}"</f>
+        <v>      , {"rank": 46, "name": "Kingdom", "contribution": 41143753}</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="11" t="n">
+        <v>47</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="12" t="n">
+        <v>39936512</v>
+      </c>
+      <c r="E50" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B50&amp;", ""name"": """&amp;C50&amp;""", ""contribution"": "&amp;D50&amp;"}"</f>
+        <v>      , {"rank": 47, "name": "Reboot", "contribution": 39936512}</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="11" t="n">
+        <v>48</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D51" s="12" t="n">
+        <v>39638954</v>
+      </c>
+      <c r="E51" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B51&amp;", ""name"": """&amp;C51&amp;""", ""contribution"": "&amp;D51&amp;"}"</f>
+        <v>      , {"rank": 48, "name": "Exorcist", "contribution": 39638954}</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="11" t="n">
+        <v>49</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="12" t="n">
+        <v>38974765</v>
+      </c>
+      <c r="E52" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B52&amp;", ""name"": """&amp;C52&amp;""", ""contribution"": "&amp;D52&amp;"}"</f>
+        <v>      , {"rank": 49, "name": "Faction", "contribution": 38974765}</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="11" t="n">
+        <v>50</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="12" t="n">
+        <v>36645409</v>
+      </c>
+      <c r="E53" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B53&amp;", ""name"": """&amp;C53&amp;""", ""contribution"": "&amp;D53&amp;"}"</f>
+        <v>      , {"rank": 50, "name": "Prestigious", "contribution": 36645409}</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="13" t="str">
+        <f aca="false">"    "&amp;"],"</f>
+        <v>    ],</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated monthly Honorable Rock and archive spreadsheet
</commit_message>
<xml_diff>
--- a/data/MapleStory Monthly Honorable Rock Record.xlsx
+++ b/data/MapleStory Monthly Honorable Rock Record.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="August 2019" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="September 2019" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="October 2019" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="November 2019" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="December 2019" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="55">
   <si>
     <t xml:space="preserve">Rank</t>
   </si>
@@ -185,6 +186,9 @@
   </si>
   <si>
     <t xml:space="preserve">Prestigious</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HeavenSent</t>
   </si>
 </sst>
 </file>
@@ -448,7 +452,7 @@
   <dimension ref="B1:E54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+      <selection pane="topLeft" activeCell="C49" activeCellId="0" sqref="B4:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1269,7 +1273,7 @@
   <dimension ref="B1:E54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="B4:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2090,7 +2094,7 @@
   <dimension ref="B1:E54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="1" sqref="B4:C50 E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2910,8 +2914,8 @@
   </sheetPr>
   <dimension ref="B1:E54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="B4:C50 E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3722,4 +3726,825 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:E54"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="B4:C50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="0.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="5.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="59.9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="4" customFormat="true" ht="4.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D1" s="5"/>
+      <c r="E1" s="6"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="str">
+        <f aca="false">"    """&amp;"December 2019"&amp;""""&amp;":"</f>
+        <v>    "December 2019":</v>
+      </c>
+    </row>
+    <row r="3" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="10" t="str">
+        <f aca="false">"    "&amp;"["</f>
+        <v>    [</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12" t="n">
+        <v>240789974</v>
+      </c>
+      <c r="E4" s="10" t="str">
+        <f aca="false">"      "&amp;"{""rank"": "&amp;B4&amp;", ""name"": """&amp;C4&amp;""", ""contribution"": "&amp;D4&amp;"}"</f>
+        <v>      {"rank": 1, "name": "Eternal", "contribution": 240789974}</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="12" t="n">
+        <v>230242820</v>
+      </c>
+      <c r="E5" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B5&amp;", ""name"": """&amp;C5&amp;""", ""contribution"": "&amp;D5&amp;"}"</f>
+        <v>      , {"rank": 2, "name": "Smile", "contribution": 230242820}</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="12" t="n">
+        <v>216089993</v>
+      </c>
+      <c r="E6" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B6&amp;", ""name"": """&amp;C6&amp;""", ""contribution"": "&amp;D6&amp;"}"</f>
+        <v>      , {"rank": 3, "name": "Savages", "contribution": 216089993}</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="12" t="n">
+        <v>205319584</v>
+      </c>
+      <c r="E7" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B7&amp;", ""name"": """&amp;C7&amp;""", ""contribution"": "&amp;D7&amp;"}"</f>
+        <v>      , {"rank": 4, "name": "Elite", "contribution": 205319584}</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="12" t="n">
+        <v>204399710</v>
+      </c>
+      <c r="E8" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B8&amp;", ""name"": """&amp;C8&amp;""", ""contribution"": "&amp;D8&amp;"}"</f>
+        <v>      , {"rank": 5, "name": "Bounce", "contribution": 204399710}</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="12" t="n">
+        <v>145824555</v>
+      </c>
+      <c r="E9" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B9&amp;", ""name"": """&amp;C9&amp;""", ""contribution"": "&amp;D9&amp;"}"</f>
+        <v>      , {"rank": 6, "name": "Spring", "contribution": 145824555}</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="12" t="n">
+        <v>136931011</v>
+      </c>
+      <c r="E10" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B10&amp;", ""name"": """&amp;C10&amp;""", ""contribution"": "&amp;D10&amp;"}"</f>
+        <v>      , {"rank": 7, "name": "Sunset", "contribution": 136931011}</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="12" t="n">
+        <v>126046520</v>
+      </c>
+      <c r="E11" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B11&amp;", ""name"": """&amp;C11&amp;""", ""contribution"": "&amp;D11&amp;"}"</f>
+        <v>      , {"rank": 8, "name": "Epic", "contribution": 126046520}</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="12" t="n">
+        <v>118695090</v>
+      </c>
+      <c r="E12" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B12&amp;", ""name"": """&amp;C12&amp;""", ""contribution"": "&amp;D12&amp;"}"</f>
+        <v>      , {"rank": 9, "name": "Beaters", "contribution": 118695090}</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="12" t="n">
+        <v>116795406</v>
+      </c>
+      <c r="E13" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B13&amp;", ""name"": """&amp;C13&amp;""", ""contribution"": "&amp;D13&amp;"}"</f>
+        <v>      , {"rank": 10, "name": "Downtime", "contribution": 116795406}</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="12" t="n">
+        <v>99533446</v>
+      </c>
+      <c r="E14" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B14&amp;", ""name"": """&amp;C14&amp;""", ""contribution"": "&amp;D14&amp;"}"</f>
+        <v>      , {"rank": 11, "name": "RainSong", "contribution": 99533446}</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="12" t="n">
+        <v>98658827</v>
+      </c>
+      <c r="E15" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B15&amp;", ""name"": """&amp;C15&amp;""", ""contribution"": "&amp;D15&amp;"}"</f>
+        <v>      , {"rank": 12, "name": "lolicafe", "contribution": 98658827}</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="11" t="n">
+        <v>13</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="12" t="n">
+        <v>97872638</v>
+      </c>
+      <c r="E16" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B16&amp;", ""name"": """&amp;C16&amp;""", ""contribution"": "&amp;D16&amp;"}"</f>
+        <v>      , {"rank": 13, "name": "Imperium", "contribution": 97872638}</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="11" t="n">
+        <v>14</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="12" t="n">
+        <v>87349880</v>
+      </c>
+      <c r="E17" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B17&amp;", ""name"": """&amp;C17&amp;""", ""contribution"": "&amp;D17&amp;"}"</f>
+        <v>      , {"rank": 14, "name": "Gintama", "contribution": 87349880}</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="12" t="n">
+        <v>86638324</v>
+      </c>
+      <c r="E18" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B18&amp;", ""name"": """&amp;C18&amp;""", ""contribution"": "&amp;D18&amp;"}"</f>
+        <v>      , {"rank": 15, "name": "Undertale", "contribution": 86638324}</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="11" t="n">
+        <v>16</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="12" t="n">
+        <v>85337314</v>
+      </c>
+      <c r="E19" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B19&amp;", ""name"": """&amp;C19&amp;""", ""contribution"": "&amp;D19&amp;"}"</f>
+        <v>      , {"rank": 16, "name": "Maha", "contribution": 85337314}</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="11" t="n">
+        <v>17</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="12" t="n">
+        <v>85244997</v>
+      </c>
+      <c r="E20" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B20&amp;", ""name"": """&amp;C20&amp;""", ""contribution"": "&amp;D20&amp;"}"</f>
+        <v>      , {"rank": 17, "name": "Remorse", "contribution": 85244997}</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="11" t="n">
+        <v>18</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="12" t="n">
+        <v>81758022</v>
+      </c>
+      <c r="E21" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B21&amp;", ""name"": """&amp;C21&amp;""", ""contribution"": "&amp;D21&amp;"}"</f>
+        <v>      , {"rank": 18, "name": "Erda", "contribution": 81758022}</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="11" t="n">
+        <v>19</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="12" t="n">
+        <v>80272929</v>
+      </c>
+      <c r="E22" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B22&amp;", ""name"": """&amp;C22&amp;""", ""contribution"": "&amp;D22&amp;"}"</f>
+        <v>      , {"rank": 19, "name": "Cleanse", "contribution": 80272929}</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="12" t="n">
+        <v>79019826</v>
+      </c>
+      <c r="E23" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B23&amp;", ""name"": """&amp;C23&amp;""", ""contribution"": "&amp;D23&amp;"}"</f>
+        <v>      , {"rank": 20, "name": "Atelier", "contribution": 79019826}</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="11" t="n">
+        <v>21</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="12" t="n">
+        <v>75775892</v>
+      </c>
+      <c r="E24" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B24&amp;", ""name"": """&amp;C24&amp;""", ""contribution"": "&amp;D24&amp;"}"</f>
+        <v>      , {"rank": 21, "name": "Broke", "contribution": 75775892}</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="11" t="n">
+        <v>22</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="12" t="n">
+        <v>75631668</v>
+      </c>
+      <c r="E25" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B25&amp;", ""name"": """&amp;C25&amp;""", ""contribution"": "&amp;D25&amp;"}"</f>
+        <v>      , {"rank": 22, "name": "Sora", "contribution": 75631668}</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="11" t="n">
+        <v>23</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="12" t="n">
+        <v>74979459</v>
+      </c>
+      <c r="E26" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B26&amp;", ""name"": """&amp;C26&amp;""", ""contribution"": "&amp;D26&amp;"}"</f>
+        <v>      , {"rank": 23, "name": "Tama", "contribution": 74979459}</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="11" t="n">
+        <v>24</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="12" t="n">
+        <v>69131473</v>
+      </c>
+      <c r="E27" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B27&amp;", ""name"": """&amp;C27&amp;""", ""contribution"": "&amp;D27&amp;"}"</f>
+        <v>      , {"rank": 24, "name": "Lithe", "contribution": 69131473}</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="12" t="n">
+        <v>69012616</v>
+      </c>
+      <c r="E28" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B28&amp;", ""name"": """&amp;C28&amp;""", ""contribution"": "&amp;D28&amp;"}"</f>
+        <v>      , {"rank": 25, "name": "Oceania", "contribution": 69012616}</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="11" t="n">
+        <v>26</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="12" t="n">
+        <v>68318091</v>
+      </c>
+      <c r="E29" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B29&amp;", ""name"": """&amp;C29&amp;""", ""contribution"": "&amp;D29&amp;"}"</f>
+        <v>      , {"rank": 26, "name": "Revive", "contribution": 68318091}</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="11" t="n">
+        <v>27</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D30" s="12" t="n">
+        <v>64206429</v>
+      </c>
+      <c r="E30" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B30&amp;", ""name"": """&amp;C30&amp;""", ""contribution"": "&amp;D30&amp;"}"</f>
+        <v>      , {"rank": 27, "name": "Rising", "contribution": 64206429}</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="11" t="n">
+        <v>28</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="12" t="n">
+        <v>62783449</v>
+      </c>
+      <c r="E31" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B31&amp;", ""name"": """&amp;C31&amp;""", ""contribution"": "&amp;D31&amp;"}"</f>
+        <v>      , {"rank": 28, "name": "Ravers", "contribution": 62783449}</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="11" t="n">
+        <v>29</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="12" t="n">
+        <v>62760688</v>
+      </c>
+      <c r="E32" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B32&amp;", ""name"": """&amp;C32&amp;""", ""contribution"": "&amp;D32&amp;"}"</f>
+        <v>      , {"rank": 29, "name": "Sugar", "contribution": 62760688}</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="11" t="n">
+        <v>30</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="12" t="n">
+        <v>61609928</v>
+      </c>
+      <c r="E33" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B33&amp;", ""name"": """&amp;C33&amp;""", ""contribution"": "&amp;D33&amp;"}"</f>
+        <v>      , {"rank": 30, "name": "Artifacts", "contribution": 61609928}</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="11" t="n">
+        <v>31</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="12" t="n">
+        <v>56077460</v>
+      </c>
+      <c r="E34" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B34&amp;", ""name"": """&amp;C34&amp;""", ""contribution"": "&amp;D34&amp;"}"</f>
+        <v>      , {"rank": 31, "name": "Fabled", "contribution": 56077460}</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="11" t="n">
+        <v>32</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" s="12" t="n">
+        <v>55086052</v>
+      </c>
+      <c r="E35" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B35&amp;", ""name"": """&amp;C35&amp;""", ""contribution"": "&amp;D35&amp;"}"</f>
+        <v>      , {"rank": 32, "name": "Aloe", "contribution": 55086052}</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="11" t="n">
+        <v>33</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="12" t="n">
+        <v>54168958</v>
+      </c>
+      <c r="E36" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B36&amp;", ""name"": """&amp;C36&amp;""", ""contribution"": "&amp;D36&amp;"}"</f>
+        <v>      , {"rank": 33, "name": "Earnest", "contribution": 54168958}</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="11" t="n">
+        <v>34</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="12" t="n">
+        <v>51007455</v>
+      </c>
+      <c r="E37" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B37&amp;", ""name"": """&amp;C37&amp;""", ""contribution"": "&amp;D37&amp;"}"</f>
+        <v>      , {"rank": 34, "name": "Skyfall", "contribution": 51007455}</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="11" t="n">
+        <v>35</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="12" t="n">
+        <v>49821525</v>
+      </c>
+      <c r="E38" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B38&amp;", ""name"": """&amp;C38&amp;""", ""contribution"": "&amp;D38&amp;"}"</f>
+        <v>      , {"rank": 35, "name": "CyberThreat", "contribution": 49821525}</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="11" t="n">
+        <v>36</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="12" t="n">
+        <v>49764060</v>
+      </c>
+      <c r="E39" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B39&amp;", ""name"": """&amp;C39&amp;""", ""contribution"": "&amp;D39&amp;"}"</f>
+        <v>      , {"rank": 36, "name": "Mystical", "contribution": 49764060}</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="11" t="n">
+        <v>37</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="12" t="n">
+        <v>48676027</v>
+      </c>
+      <c r="E40" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B40&amp;", ""name"": """&amp;C40&amp;""", ""contribution"": "&amp;D40&amp;"}"</f>
+        <v>      , {"rank": 37, "name": "chigga", "contribution": 48676027}</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="11" t="n">
+        <v>38</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41" s="12" t="n">
+        <v>47515495</v>
+      </c>
+      <c r="E41" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B41&amp;", ""name"": """&amp;C41&amp;""", ""contribution"": "&amp;D41&amp;"}"</f>
+        <v>      , {"rank": 38, "name": "Fandom", "contribution": 47515495}</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="11" t="n">
+        <v>39</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" s="12" t="n">
+        <v>46461256</v>
+      </c>
+      <c r="E42" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B42&amp;", ""name"": """&amp;C42&amp;""", ""contribution"": "&amp;D42&amp;"}"</f>
+        <v>      , {"rank": 39, "name": "Howl", "contribution": 46461256}</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="11" t="n">
+        <v>40</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D43" s="12" t="n">
+        <v>45174624</v>
+      </c>
+      <c r="E43" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B43&amp;", ""name"": """&amp;C43&amp;""", ""contribution"": "&amp;D43&amp;"}"</f>
+        <v>      , {"rank": 40, "name": "RainDrop", "contribution": 45174624}</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="11" t="n">
+        <v>41</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="12" t="n">
+        <v>44934426</v>
+      </c>
+      <c r="E44" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B44&amp;", ""name"": """&amp;C44&amp;""", ""contribution"": "&amp;D44&amp;"}"</f>
+        <v>      , {"rank": 41, "name": "Path", "contribution": 44934426}</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="11" t="n">
+        <v>42</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="12" t="n">
+        <v>42810639</v>
+      </c>
+      <c r="E45" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B45&amp;", ""name"": """&amp;C45&amp;""", ""contribution"": "&amp;D45&amp;"}"</f>
+        <v>      , {"rank": 42, "name": "Bubbles", "contribution": 42810639}</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="11" t="n">
+        <v>43</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="12" t="n">
+        <v>42294515</v>
+      </c>
+      <c r="E46" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B46&amp;", ""name"": """&amp;C46&amp;""", ""contribution"": "&amp;D46&amp;"}"</f>
+        <v>      , {"rank": 43, "name": "Coffee", "contribution": 42294515}</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="11" t="n">
+        <v>44</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D47" s="12" t="n">
+        <v>41908988</v>
+      </c>
+      <c r="E47" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B47&amp;", ""name"": """&amp;C47&amp;""", ""contribution"": "&amp;D47&amp;"}"</f>
+        <v>      , {"rank": 44, "name": "Weibo", "contribution": 41908988}</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="11" t="n">
+        <v>45</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D48" s="12" t="n">
+        <v>41757438</v>
+      </c>
+      <c r="E48" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B48&amp;", ""name"": """&amp;C48&amp;""", ""contribution"": "&amp;D48&amp;"}"</f>
+        <v>      , {"rank": 45, "name": "Kingdom", "contribution": 41757438}</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="11" t="n">
+        <v>46</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" s="12" t="n">
+        <v>41161676</v>
+      </c>
+      <c r="E49" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B49&amp;", ""name"": """&amp;C49&amp;""", ""contribution"": "&amp;D49&amp;"}"</f>
+        <v>      , {"rank": 46, "name": "Exorcist", "contribution": 41161676}</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="11" t="n">
+        <v>47</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="12" t="n">
+        <v>40474527</v>
+      </c>
+      <c r="E50" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B50&amp;", ""name"": """&amp;C50&amp;""", ""contribution"": "&amp;D50&amp;"}"</f>
+        <v>      , {"rank": 47, "name": "Reboot", "contribution": 40474527}</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="11" t="n">
+        <v>48</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="12" t="n">
+        <v>40296928</v>
+      </c>
+      <c r="E51" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B51&amp;", ""name"": """&amp;C51&amp;""", ""contribution"": "&amp;D51&amp;"}"</f>
+        <v>      , {"rank": 48, "name": "Comity", "contribution": 40296928}</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="11" t="n">
+        <v>49</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D52" s="12" t="n">
+        <v>39639099</v>
+      </c>
+      <c r="E52" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B52&amp;", ""name"": """&amp;C52&amp;""", ""contribution"": "&amp;D52&amp;"}"</f>
+        <v>      , {"rank": 49, "name": "Faction", "contribution": 39639099}</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="11" t="n">
+        <v>50</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D53" s="12" t="n">
+        <v>37046670</v>
+      </c>
+      <c r="E53" s="10" t="str">
+        <f aca="false">"      "&amp;", {""rank"": "&amp;B53&amp;", ""name"": """&amp;C53&amp;""", ""contribution"": "&amp;D53&amp;"}"</f>
+        <v>      , {"rank": 50, "name": "HeavenSent", "contribution": 37046670}</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="13" t="str">
+        <f aca="false">"    "&amp;"],"</f>
+        <v>    ],</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>